<commit_message>
added new assets from matchsync-ig
</commit_message>
<xml_diff>
--- a/CodeSystem-glstring-codesystem.xlsx
+++ b/CodeSystem-glstring-codesystem.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
   <si>
     <t>Property</t>
   </si>
@@ -53,10 +53,13 @@
     <t>Experimental</t>
   </si>
   <si>
+    <t>true</t>
+  </si>
+  <si>
     <t>Date</t>
   </si>
   <si>
-    <t>2022-11-02T14:44:07-05:00</t>
+    <t>2024-02-19T18:37:26-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -96,9 +99,6 @@
   </si>
   <si>
     <t>Compositional</t>
-  </si>
-  <si>
-    <t>true</t>
   </si>
   <si>
     <t>Version Needed?</t>
@@ -235,10 +235,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyFont="true">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyBorder="true" applyFill="true" applyAlignment="true" applyFont="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="true" applyAlignment="true">
       <alignment vertical="top" wrapText="true"/>
     </xf>
   </cellXfs>
@@ -309,78 +309,82 @@
       <c r="A7" t="s" s="2">
         <v>12</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B11" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B12" s="2"/>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="B14" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="B14" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B15" s="2"/>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>28</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18">

</xml_diff>

<commit_message>
Update for release to deply 0.1.1
</commit_message>
<xml_diff>
--- a/CodeSystem-glstring-codesystem.xlsx
+++ b/CodeSystem-glstring-codesystem.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
   <si>
     <t>Property</t>
   </si>
@@ -29,7 +29,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>0.1.1</t>
   </si>
   <si>
     <t>Name</t>
@@ -59,7 +59,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-05-20T10:22:59-05:00</t>
+    <t>2024-11-11T17:53:38-06:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>NMDP (http://bethematch.org)</t>
+  </si>
+  <si>
+    <t>Jurisdiction</t>
+  </si>
+  <si>
+    <t/>
   </si>
   <si>
     <t>Description</t>
@@ -247,7 +253,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B21"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -349,69 +355,77 @@
       <c r="A12" t="s" s="2">
         <v>22</v>
       </c>
-      <c r="B12" s="2"/>
+      <c r="B12" t="s" s="2">
+        <v>23</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="2">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s" s="2">
         <v>24</v>
       </c>
+      <c r="B13" s="2"/>
     </row>
     <row r="14">
       <c r="A14" t="s" s="2">
         <v>25</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="2">
-        <v>26</v>
-      </c>
-      <c r="B15" s="2"/>
+        <v>27</v>
+      </c>
+      <c r="B15" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" s="2"/>
     </row>
     <row r="17">
       <c r="A17" t="s" s="2">
-        <v>28</v>
-      </c>
-      <c r="B17" t="s" s="2">
-        <v>13</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="B17" s="2"/>
     </row>
     <row r="18">
       <c r="A18" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="B18" s="2"/>
+        <v>30</v>
+      </c>
+      <c r="B18" t="s" s="2">
+        <v>13</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s" s="2">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s" s="2">
         <v>31</v>
       </c>
+      <c r="B19" s="2"/>
     </row>
     <row r="20">
       <c r="A20" t="s" s="2">
         <v>32</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" t="s" s="2">
+        <v>33</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="2">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s" s="2">
+        <v>35</v>
+      </c>
+      <c r="B22" s="2"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>